<commit_message>
Versión copieditada Recurso nuevo reemplaza al archivo pendiente de borrar
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/esqueletoGuion_CS_07_02.xlsx
+++ b/fuentes/contenidos/grado07/guion02/esqueletoGuion_CS_07_02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23120" windowHeight="13400" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23120" windowHeight="13400" tabRatio="729" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="130">
   <si>
     <t>FICHA</t>
   </si>
@@ -423,6 +423,11 @@
   </si>
   <si>
     <t>El feudo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autoevaluación
+Evalúa tus conocimientos sobre el tema del feudalismo
+</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2045,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2943,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2965,9 +2970,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="15">
-      <c r="A2" s="14" t="s">
-        <v>23</v>
+    <row r="2" spans="1:3" s="4" customFormat="1" ht="90">
+      <c r="A2" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>68</v>
@@ -3510,7 +3515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H136" sqref="H136"/>
     </sheetView>

</xml_diff>